<commit_message>
Add files via upload (#114)
I I have changed the name of the file so that it matches the file it is supposed to replace.
You can remove the file called: BRIK cabinets_ availability, location and how to use.xlsx. I cannot delete it my self.
Then I hope I succeed in getting the updated version linked to the website
</commit_message>
<xml_diff>
--- a/files/brik-cabinets.xlsx
+++ b/files/brik-cabinets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\HE_CLIN-Biokemisk-Patologi\0 SDCA Forskning_Jessen Group\0 Velkommen på plan 4_SDCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE8BD00-D950-4E39-8D5A-944DDE734724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7335036F-81B2-4990-A214-5A6837374BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="424">
   <si>
     <t>Cabinet</t>
   </si>
@@ -1354,7 +1354,19 @@
     <t>as they are non-stock items.</t>
   </si>
   <si>
-    <t>27.June-2024</t>
+    <t>Frysepose, 6L / 50cmx25cm</t>
+  </si>
+  <si>
+    <t>6L</t>
+  </si>
+  <si>
+    <t>20m x 29cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alufolie </t>
+  </si>
+  <si>
+    <t>14.Jan-2025</t>
   </si>
 </sst>
 </file>
@@ -5459,11 +5471,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M198"/>
+  <dimension ref="A1:M200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O158" sqref="O158"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5476,7 +5488,7 @@
     <col min="6" max="6" width="7.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="5" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" style="15" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" style="2"/>
     <col min="12" max="12" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -5522,7 +5534,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10445,143 +10457,143 @@
       </c>
       <c r="J168" s="48"/>
     </row>
-    <row r="169" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="22">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" s="31">
         <v>446</v>
       </c>
-      <c r="B169" s="23">
+      <c r="B169" s="32">
         <v>7</v>
       </c>
-      <c r="C169" s="23" t="s">
+      <c r="C169" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="D169" s="24" t="s">
+      <c r="D169" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="E169" s="24" t="s">
+      <c r="E169" s="33" t="s">
         <v>295</v>
       </c>
-      <c r="F169" s="23">
-        <v>1</v>
-      </c>
-      <c r="G169" s="23" t="s">
+      <c r="F169" s="32">
+        <v>1</v>
+      </c>
+      <c r="G169" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H169" s="23">
+      <c r="H169" s="32">
         <v>1032263</v>
       </c>
-      <c r="I169" s="25">
+      <c r="I169" s="34">
         <v>57</v>
       </c>
-      <c r="J169" s="49"/>
+      <c r="J169" s="48"/>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A170" s="16">
+      <c r="A170" s="31">
+        <v>446</v>
+      </c>
+      <c r="B170" s="32">
+        <v>8</v>
+      </c>
+      <c r="C170" s="32">
+        <v>10812846</v>
+      </c>
+      <c r="D170" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="E170" s="33" t="s">
+        <v>420</v>
+      </c>
+      <c r="F170" s="32">
+        <v>1</v>
+      </c>
+      <c r="G170" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H170" s="32">
+        <v>1064720</v>
+      </c>
+      <c r="I170" s="34">
+        <v>0.12</v>
+      </c>
+      <c r="J170" s="48"/>
+    </row>
+    <row r="171" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="22">
+        <v>446</v>
+      </c>
+      <c r="B171" s="23">
+        <v>8</v>
+      </c>
+      <c r="C171" s="23">
+        <v>30043824</v>
+      </c>
+      <c r="D171" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="E171" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="F171" s="23">
+        <v>10</v>
+      </c>
+      <c r="G171" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H171" s="23">
+        <v>1064721</v>
+      </c>
+      <c r="I171" s="25">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="J171" s="49"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" s="16">
         <v>447</v>
       </c>
-      <c r="B170" s="17">
-        <v>1</v>
-      </c>
-      <c r="C170" s="17" t="s">
+      <c r="B172" s="17">
+        <v>1</v>
+      </c>
+      <c r="C172" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="D170" s="18" t="s">
+      <c r="D172" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="E170" s="18" t="s">
+      <c r="E172" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="F170" s="17">
-        <v>1</v>
-      </c>
-      <c r="G170" s="17" t="s">
+      <c r="F172" s="17">
+        <v>1</v>
+      </c>
+      <c r="G172" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H170" s="17">
+      <c r="H172" s="17">
         <v>1034955</v>
       </c>
-      <c r="I170" s="19">
+      <c r="I172" s="19">
         <v>24</v>
       </c>
-      <c r="J170" s="50" t="s">
+      <c r="J172" s="50" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A171" s="20">
-        <v>447</v>
-      </c>
-      <c r="B171" s="9">
-        <v>1</v>
-      </c>
-      <c r="C171" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D171" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="E171" s="10">
-        <v>11</v>
-      </c>
-      <c r="F171" s="9">
-        <v>1</v>
-      </c>
-      <c r="G171" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H171" s="9">
-        <v>1034954</v>
-      </c>
-      <c r="I171" s="21">
-        <v>34.4</v>
-      </c>
-      <c r="J171" s="48"/>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A172" s="20">
-        <v>447</v>
-      </c>
-      <c r="B172" s="9">
-        <v>1</v>
-      </c>
-      <c r="C172" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="D172" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="E172" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="F172" s="9">
-        <v>1</v>
-      </c>
-      <c r="G172" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H172" s="9">
-        <v>1032672</v>
-      </c>
-      <c r="I172" s="21">
-        <v>22.74</v>
-      </c>
-      <c r="J172" s="48"/>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="20">
         <v>447</v>
       </c>
       <c r="B173" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="E173" s="10" t="s">
-        <v>245</v>
+        <v>219</v>
+      </c>
+      <c r="E173" s="10">
+        <v>11</v>
       </c>
       <c r="F173" s="9">
         <v>1</v>
@@ -10590,10 +10602,10 @@
         <v>12</v>
       </c>
       <c r="H173" s="9">
-        <v>1034956</v>
+        <v>1034954</v>
       </c>
       <c r="I173" s="21">
-        <v>30</v>
+        <v>34.4</v>
       </c>
       <c r="J173" s="48"/>
     </row>
@@ -10602,16 +10614,16 @@
         <v>447</v>
       </c>
       <c r="B174" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E174" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F174" s="9">
         <v>1</v>
@@ -10620,10 +10632,10 @@
         <v>12</v>
       </c>
       <c r="H174" s="9">
-        <v>1032671</v>
+        <v>1032672</v>
       </c>
       <c r="I174" s="21">
-        <v>127.2</v>
+        <v>22.74</v>
       </c>
       <c r="J174" s="48"/>
     </row>
@@ -10632,26 +10644,28 @@
         <v>447</v>
       </c>
       <c r="B175" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="E175" s="10"/>
+        <v>244</v>
+      </c>
+      <c r="E175" s="10" t="s">
+        <v>245</v>
+      </c>
       <c r="F175" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G175" s="9" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="H175" s="9">
-        <v>1032658</v>
+        <v>1034956</v>
       </c>
       <c r="I175" s="21">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J175" s="48"/>
     </row>
@@ -10660,28 +10674,28 @@
         <v>447</v>
       </c>
       <c r="B176" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>269</v>
+        <v>299</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="E176" s="10" t="s">
-        <v>271</v>
+        <v>301</v>
       </c>
       <c r="F176" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G176" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H176" s="9">
-        <v>1032659</v>
+        <v>1032671</v>
       </c>
       <c r="I176" s="21">
-        <v>42</v>
+        <v>127.2</v>
       </c>
       <c r="J176" s="48"/>
     </row>
@@ -10690,26 +10704,26 @@
         <v>447</v>
       </c>
       <c r="B177" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>222</v>
+        <v>272</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>223</v>
+        <v>273</v>
       </c>
       <c r="E177" s="10"/>
       <c r="F177" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G177" s="9" t="s">
         <v>157</v>
       </c>
       <c r="H177" s="9">
-        <v>1032660</v>
+        <v>1032658</v>
       </c>
       <c r="I177" s="21">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="J177" s="48"/>
     </row>
@@ -10718,26 +10732,28 @@
         <v>447</v>
       </c>
       <c r="B178" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>302</v>
+        <v>269</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="E178" s="10"/>
+        <v>270</v>
+      </c>
+      <c r="E178" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="F178" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G178" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H178" s="9">
-        <v>1032661</v>
+        <v>1032659</v>
       </c>
       <c r="I178" s="21">
-        <v>1496.21</v>
+        <v>42</v>
       </c>
       <c r="J178" s="48"/>
     </row>
@@ -10746,26 +10762,26 @@
         <v>447</v>
       </c>
       <c r="B179" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>21</v>
+        <v>223</v>
       </c>
       <c r="E179" s="10"/>
       <c r="F179" s="9">
         <v>1</v>
       </c>
       <c r="G179" s="9" t="s">
-        <v>15</v>
+        <v>157</v>
       </c>
       <c r="H179" s="9">
-        <v>1032662</v>
+        <v>1032660</v>
       </c>
       <c r="I179" s="21">
-        <v>865.1</v>
+        <v>83</v>
       </c>
       <c r="J179" s="48"/>
     </row>
@@ -10774,26 +10790,26 @@
         <v>447</v>
       </c>
       <c r="B180" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>16</v>
+        <v>302</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>17</v>
+        <v>303</v>
       </c>
       <c r="E180" s="10"/>
-      <c r="F180" s="9" t="s">
-        <v>18</v>
+      <c r="F180" s="9">
+        <v>1</v>
       </c>
       <c r="G180" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H180" s="9">
-        <v>1032663</v>
+        <v>1032661</v>
       </c>
       <c r="I180" s="21">
-        <v>0.49</v>
+        <v>1496.21</v>
       </c>
       <c r="J180" s="48"/>
     </row>
@@ -10802,13 +10818,13 @@
         <v>447</v>
       </c>
       <c r="B181" s="9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E181" s="10"/>
       <c r="F181" s="9">
@@ -10818,68 +10834,66 @@
         <v>15</v>
       </c>
       <c r="H181" s="9">
-        <v>1035358</v>
+        <v>1032662</v>
       </c>
       <c r="I181" s="21">
-        <v>956.1</v>
+        <v>865.1</v>
       </c>
       <c r="J181" s="48"/>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="20">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B182" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>293</v>
+        <v>16</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="E182" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="F182" s="9">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="E182" s="10"/>
+      <c r="F182" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="G182" s="9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H182" s="9">
-        <v>1032673</v>
+        <v>1032663</v>
       </c>
       <c r="I182" s="21">
-        <v>57</v>
+        <v>0.49</v>
       </c>
       <c r="J182" s="48"/>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="20">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B183" s="9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>304</v>
+        <v>13</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>305</v>
+        <v>14</v>
       </c>
       <c r="E183" s="10"/>
       <c r="F183" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G183" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H183" s="9">
-        <v>1033048</v>
+        <v>1035358</v>
       </c>
       <c r="I183" s="21">
-        <v>33.53</v>
+        <v>956.1</v>
       </c>
       <c r="J183" s="48"/>
     </row>
@@ -10888,28 +10902,28 @@
         <v>448</v>
       </c>
       <c r="B184" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="E184" s="10" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="F184" s="9">
         <v>1</v>
       </c>
       <c r="G184" s="9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H184" s="9">
-        <v>1032676</v>
+        <v>1032673</v>
       </c>
       <c r="I184" s="21">
-        <v>179.81</v>
+        <v>57</v>
       </c>
       <c r="J184" s="48"/>
     </row>
@@ -10918,28 +10932,26 @@
         <v>448</v>
       </c>
       <c r="B185" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>180</v>
+        <v>304</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E185" s="10" t="s">
-        <v>182</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="E185" s="10"/>
       <c r="F185" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G185" s="9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H185" s="9">
-        <v>1032677</v>
+        <v>1033048</v>
       </c>
       <c r="I185" s="21">
-        <v>0</v>
+        <v>33.53</v>
       </c>
       <c r="J185" s="48"/>
     </row>
@@ -10948,28 +10960,28 @@
         <v>448</v>
       </c>
       <c r="B186" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>177</v>
+        <v>306</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>178</v>
+        <v>307</v>
       </c>
       <c r="E186" s="10" t="s">
-        <v>179</v>
+        <v>308</v>
       </c>
       <c r="F186" s="9">
         <v>1</v>
       </c>
       <c r="G186" s="9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H186" s="9">
-        <v>1032678</v>
+        <v>1032676</v>
       </c>
       <c r="I186" s="21">
-        <v>0</v>
+        <v>179.81</v>
       </c>
       <c r="J186" s="48"/>
     </row>
@@ -10981,13 +10993,13 @@
         <v>8</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E187" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F187" s="9">
         <v>1</v>
@@ -10996,7 +11008,7 @@
         <v>12</v>
       </c>
       <c r="H187" s="9">
-        <v>1032679</v>
+        <v>1032677</v>
       </c>
       <c r="I187" s="21">
         <v>0</v>
@@ -11008,15 +11020,17 @@
         <v>448</v>
       </c>
       <c r="B188" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>291</v>
+        <v>177</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="E188" s="10"/>
+        <v>178</v>
+      </c>
+      <c r="E188" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="F188" s="9">
         <v>1</v>
       </c>
@@ -11024,10 +11038,10 @@
         <v>12</v>
       </c>
       <c r="H188" s="9">
-        <v>1032680</v>
+        <v>1032678</v>
       </c>
       <c r="I188" s="21">
-        <v>196.17</v>
+        <v>0</v>
       </c>
       <c r="J188" s="48"/>
     </row>
@@ -11036,89 +11050,147 @@
         <v>448</v>
       </c>
       <c r="B189" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>29</v>
+        <v>183</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
       <c r="E189" s="10" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="F189" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G189" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H189" s="9">
+        <v>1032679</v>
+      </c>
+      <c r="I189" s="21">
+        <v>0</v>
+      </c>
+      <c r="J189" s="48"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" s="20">
+        <v>448</v>
+      </c>
+      <c r="B190" s="9">
+        <v>9</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="D190" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="E190" s="10"/>
+      <c r="F190" s="9">
+        <v>1</v>
+      </c>
+      <c r="G190" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H190" s="9">
+        <v>1032680</v>
+      </c>
+      <c r="I190" s="21">
+        <v>196.17</v>
+      </c>
+      <c r="J190" s="48"/>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" s="20">
+        <v>448</v>
+      </c>
+      <c r="B191" s="9">
+        <v>9</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D191" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E191" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F191" s="9">
+        <v>2</v>
+      </c>
+      <c r="G191" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H191" s="9">
         <v>1032681</v>
       </c>
-      <c r="I189" s="21">
+      <c r="I191" s="21">
         <v>13.75</v>
       </c>
-      <c r="J189" s="48"/>
-    </row>
-    <row r="190" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="22">
+      <c r="J191" s="48"/>
+    </row>
+    <row r="192" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="22">
         <v>448</v>
       </c>
-      <c r="B190" s="23">
+      <c r="B192" s="23">
         <v>9</v>
       </c>
-      <c r="C190" s="23" t="s">
+      <c r="C192" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D190" s="24" t="s">
+      <c r="D192" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E190" s="24" t="s">
+      <c r="E192" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F190" s="23">
+      <c r="F192" s="23">
         <v>2</v>
       </c>
-      <c r="G190" s="23" t="s">
+      <c r="G192" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H190" s="23">
+      <c r="H192" s="23">
         <v>1032682</v>
       </c>
-      <c r="I190" s="25">
+      <c r="I192" s="25">
         <v>9.5</v>
       </c>
-      <c r="J190" s="49"/>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J191" s="14"/>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J192" s="14"/>
-    </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J192" s="49"/>
+    </row>
+    <row r="193" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="J193" s="14"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="J194" s="14"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="J195" s="14"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="J196" s="14"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="J197" s="14"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="J198" s="14"/>
+    </row>
+    <row r="199" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="J199" s="14"/>
+    </row>
+    <row r="200" spans="10:10" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="J200" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="10">
-    <mergeCell ref="J170:J190"/>
+    <mergeCell ref="J172:J192"/>
     <mergeCell ref="J21:J25"/>
     <mergeCell ref="J26:J74"/>
     <mergeCell ref="J75:J104"/>
@@ -11127,7 +11199,7 @@
     <mergeCell ref="J130:J142"/>
     <mergeCell ref="J143:J148"/>
     <mergeCell ref="J149:J166"/>
-    <mergeCell ref="J167:J169"/>
+    <mergeCell ref="J167:J171"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>